<commit_message>
added map support (primative) and accounted for lowres screenshots
</commit_message>
<xml_diff>
--- a/images/output.xlsx
+++ b/images/output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -390,10 +390,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BK5"/>
+  <dimension ref="A1:BK6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="BL1" sqref="BL1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -404,20 +404,20 @@
     <col width="12.5703125" bestFit="1" customWidth="1" min="7" max="7"/>
     <col width="17.140625" customWidth="1" min="8" max="8"/>
     <col width="16.5703125" customWidth="1" min="9" max="9"/>
-    <col width="19.42578125" customWidth="1" min="10" max="10"/>
-    <col width="12.140625" customWidth="1" min="11" max="11"/>
-    <col width="16.140625" customWidth="1" min="12" max="12"/>
-    <col width="17" customWidth="1" min="13" max="13"/>
-    <col width="18.85546875" customWidth="1" min="14" max="14"/>
+    <col width="12.140625" customWidth="1" min="10" max="10"/>
+    <col width="16.140625" customWidth="1" min="11" max="11"/>
+    <col width="17" customWidth="1" min="12" max="12"/>
+    <col width="18.85546875" customWidth="1" min="13" max="13"/>
+    <col width="19.42578125" customWidth="1" min="14" max="14"/>
     <col width="17" bestFit="1" customWidth="1" min="15" max="15"/>
-    <col width="13.140625" bestFit="1" customWidth="1" min="16" max="16"/>
-    <col width="16" bestFit="1" customWidth="1" min="17" max="17"/>
-    <col width="10.85546875" bestFit="1" customWidth="1" min="18" max="18"/>
-    <col width="14.5703125" bestFit="1" customWidth="1" min="19" max="19"/>
-    <col width="14.7109375" bestFit="1" customWidth="1" min="20" max="20"/>
+    <col width="16" bestFit="1" customWidth="1" min="16" max="16"/>
+    <col width="10.85546875" bestFit="1" customWidth="1" min="17" max="17"/>
+    <col width="14.5703125" bestFit="1" customWidth="1" min="18" max="18"/>
+    <col width="14.7109375" bestFit="1" customWidth="1" min="19" max="19"/>
+    <col width="13.140625" bestFit="1" customWidth="1" min="21" max="21"/>
     <col width="17" bestFit="1" customWidth="1" min="22" max="22"/>
     <col width="16" bestFit="1" customWidth="1" min="23" max="23"/>
-    <col width="13.140625" bestFit="1" customWidth="1" min="24" max="24"/>
+    <col width="13.140625" bestFit="1" customWidth="1" min="28" max="28"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -468,29 +468,29 @@
       </c>
       <c r="J1" t="inlineStr">
         <is>
+          <t>Player 1 KA</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>Player 1 Assists</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Player 1 Deaths</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Player 1 Specials</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
           <t>Player 1 Paint</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>Player 1 KA</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>Player 1 Assists</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>Player 1 Deaths</t>
-        </is>
-      </c>
-      <c r="N1" t="inlineStr">
-        <is>
-          <t>Player 1 Specials</t>
-        </is>
-      </c>
       <c r="O1" t="inlineStr">
         <is>
           <t>Player 2 Splashtag</t>
@@ -498,34 +498,34 @@
       </c>
       <c r="P1" t="inlineStr">
         <is>
+          <t>Player 2 Weapon</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Player 2 KA</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Player 2 Assists</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Player 2 Deaths</t>
+        </is>
+      </c>
+      <c r="T1" t="inlineStr">
+        <is>
+          <t>Player 2 Specials</t>
+        </is>
+      </c>
+      <c r="U1" t="inlineStr">
+        <is>
           <t>Player 2 Paint</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
-        <is>
-          <t>Player 2 Weapon</t>
-        </is>
-      </c>
-      <c r="R1" t="inlineStr">
-        <is>
-          <t>Player 2 KA</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Player 2 Assists</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>Player 2 Deaths</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>Player 2 Specials</t>
-        </is>
-      </c>
       <c r="V1" t="inlineStr">
         <is>
           <t>Player 3 Splashtag</t>
@@ -538,29 +538,29 @@
       </c>
       <c r="X1" t="inlineStr">
         <is>
+          <t>Player 3 KA</t>
+        </is>
+      </c>
+      <c r="Y1" t="inlineStr">
+        <is>
+          <t>Player 3 Assists</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
+          <t>Player 3 Deaths</t>
+        </is>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>Player 3 Specials</t>
+        </is>
+      </c>
+      <c r="AB1" t="inlineStr">
+        <is>
           <t>Player 3 Paint</t>
         </is>
       </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>Player 3 KA</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>Player 3 Assists</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>Player 3 Deaths</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>Player 3 Specials</t>
-        </is>
-      </c>
       <c r="AC1" t="inlineStr">
         <is>
           <t>Player 4 Splashtag</t>
@@ -568,34 +568,34 @@
       </c>
       <c r="AD1" t="inlineStr">
         <is>
+          <t>Player 4 Weapon</t>
+        </is>
+      </c>
+      <c r="AE1" t="inlineStr">
+        <is>
+          <t>Player 4 KA</t>
+        </is>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>Player 4 Assists</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>Player 4 Deaths</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>Player 4 Specials</t>
+        </is>
+      </c>
+      <c r="AI1" t="inlineStr">
+        <is>
           <t>Player 4 Paint</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
-        <is>
-          <t>Player 4 Weapon</t>
-        </is>
-      </c>
-      <c r="AF1" t="inlineStr">
-        <is>
-          <t>Player 4 KA</t>
-        </is>
-      </c>
-      <c r="AG1" t="inlineStr">
-        <is>
-          <t>Player 4 Assists</t>
-        </is>
-      </c>
-      <c r="AH1" t="inlineStr">
-        <is>
-          <t>Player 4 Deaths</t>
-        </is>
-      </c>
-      <c r="AI1" t="inlineStr">
-        <is>
-          <t>Player 4 Specials</t>
-        </is>
-      </c>
       <c r="AJ1" t="inlineStr">
         <is>
           <t>Player 5 Splashtag</t>
@@ -608,29 +608,29 @@
       </c>
       <c r="AL1" t="inlineStr">
         <is>
+          <t>Player 5 KA</t>
+        </is>
+      </c>
+      <c r="AM1" t="inlineStr">
+        <is>
+          <t>Player 5 Assists</t>
+        </is>
+      </c>
+      <c r="AN1" t="inlineStr">
+        <is>
+          <t>Player 5 Deaths</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>Player 5 Specials</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
           <t>Player 5 Paint</t>
         </is>
       </c>
-      <c r="AM1" t="inlineStr">
-        <is>
-          <t>Player 5 KA</t>
-        </is>
-      </c>
-      <c r="AN1" t="inlineStr">
-        <is>
-          <t>Player 5 Assists</t>
-        </is>
-      </c>
-      <c r="AO1" t="inlineStr">
-        <is>
-          <t>Player 5 Deaths</t>
-        </is>
-      </c>
-      <c r="AP1" t="inlineStr">
-        <is>
-          <t>Player 5 Specials</t>
-        </is>
-      </c>
       <c r="AQ1" t="inlineStr">
         <is>
           <t>Player 6 Splashtag</t>
@@ -638,34 +638,34 @@
       </c>
       <c r="AR1" t="inlineStr">
         <is>
+          <t>Player 6 Weapon</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>Player 6 KA</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>Player 6 Assists</t>
+        </is>
+      </c>
+      <c r="AU1" t="inlineStr">
+        <is>
+          <t>Player 6 Deaths</t>
+        </is>
+      </c>
+      <c r="AV1" t="inlineStr">
+        <is>
+          <t>Player 6 Specials</t>
+        </is>
+      </c>
+      <c r="AW1" t="inlineStr">
+        <is>
           <t>Player 6 Paint</t>
         </is>
       </c>
-      <c r="AS1" t="inlineStr">
-        <is>
-          <t>Player 6 Weapon</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>Player 6 KA</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>Player 6 Assists</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>Player 6 Deaths</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>Player 6 Specials</t>
-        </is>
-      </c>
       <c r="AX1" t="inlineStr">
         <is>
           <t>Player 7 Splashtag</t>
@@ -678,29 +678,29 @@
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
+          <t>Player 7 KA</t>
+        </is>
+      </c>
+      <c r="BA1" t="inlineStr">
+        <is>
+          <t>Player 7 Assists</t>
+        </is>
+      </c>
+      <c r="BB1" t="inlineStr">
+        <is>
+          <t>Player 7 Deaths</t>
+        </is>
+      </c>
+      <c r="BC1" t="inlineStr">
+        <is>
+          <t>Player 7 Specials</t>
+        </is>
+      </c>
+      <c r="BD1" t="inlineStr">
+        <is>
           <t>Player 7 Paint</t>
         </is>
       </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>Player 7 KA</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>Player 7 Assists</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>Player 7 Deaths</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>Player 7 Specials</t>
-        </is>
-      </c>
       <c r="BE1" t="inlineStr">
         <is>
           <t>Player 8 Splashtag</t>
@@ -708,32 +708,32 @@
       </c>
       <c r="BF1" t="inlineStr">
         <is>
+          <t>Player 8 Weapon</t>
+        </is>
+      </c>
+      <c r="BG1" t="inlineStr">
+        <is>
+          <t>Player 8 KA</t>
+        </is>
+      </c>
+      <c r="BH1" t="inlineStr">
+        <is>
+          <t>Player 8 Assists</t>
+        </is>
+      </c>
+      <c r="BI1" t="inlineStr">
+        <is>
+          <t>Player 8 Deaths</t>
+        </is>
+      </c>
+      <c r="BJ1" t="inlineStr">
+        <is>
+          <t>Player 8 Specials</t>
+        </is>
+      </c>
+      <c r="BK1" t="inlineStr">
+        <is>
           <t>Player 8 Paint</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>Player 8 Weapon</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>Player 8 KA</t>
-        </is>
-      </c>
-      <c r="BI1" t="inlineStr">
-        <is>
-          <t>Player 8 Assists</t>
-        </is>
-      </c>
-      <c r="BJ1" t="inlineStr">
-        <is>
-          <t>Player 8 Deaths</t>
-        </is>
-      </c>
-      <c r="BK1" t="inlineStr">
-        <is>
-          <t>Player 8 Specials</t>
         </is>
       </c>
     </row>
@@ -745,7 +745,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Shipshape Cargo Co.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Inkblot Art Academy</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1379,7 +1379,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>?</t>
+          <t>Eeltail Alley</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -1696,312 +1696,594 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Scorch Gorge</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Clam Blitz</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Titans of Alterna (Orange)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>?</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Clam Blitz</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Titans of Alterna (Orange)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>CSULB Black</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>CSULB Black</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Lagoon#3554</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Inkbrush Nouveau</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>1076</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Ampri#1097</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>Heavy Edit Splatling</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>1283</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>KuroOkami☆#1988</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>Dark Tetra Dualies</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>118</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>Pinec∅ne#1756</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>Painbrush</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>1008</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>cloud#1441</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>Forge Splattershot Pro</t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="AM5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AN5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AP5" t="inlineStr">
+        <is>
+          <t>1368</t>
+        </is>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t>Deliva#2529</t>
+        </is>
+      </c>
+      <c r="AR5" t="inlineStr">
+        <is>
+          <t>Flingza Roller</t>
+        </is>
+      </c>
+      <c r="AS5" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="AT5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="AV5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AW5" t="inlineStr">
+        <is>
+          <t>899</t>
+        </is>
+      </c>
+      <c r="AX5" t="inlineStr">
+        <is>
+          <t>Dpsquirtle#1325</t>
+        </is>
+      </c>
+      <c r="AY5" t="inlineStr">
+        <is>
+          <t>Snipewriter 5H</t>
+        </is>
+      </c>
+      <c r="AZ5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BA5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="BB5" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="BC5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="BD5" t="inlineStr">
+        <is>
+          <t>1076</t>
+        </is>
+      </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>BigMan#3275</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>Splattershot</t>
+        </is>
+      </c>
+      <c r="BG5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BH5" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="BI5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="BJ5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BK5" t="inlineStr">
+        <is>
+          <t>1236</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
         <is>
           <t>?</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Lagoon#3554</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Inkbrush Nouveau</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Shipshape Cargo Co.</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Splat Zones</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Villanova Splatoon</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Ink Raiders (Bravo)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Rasta#9337</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Bamboozler 14 Mk I</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>476</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>BlazingDan#1317</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>Sloshing Machine</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>393</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>Rober#1920</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>.52 Gal</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>328</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>EstrgnBrgr#2063</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>Krak-On Splat Roller</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>1076</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Ampri#1097</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>Heavy Edit Splatling</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>397</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>AC Drift#2709</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>Dark Tetra Dualies</t>
+        </is>
+      </c>
+      <c r="AL6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AM6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AN6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="AP6" t="inlineStr">
+        <is>
+          <t>450</t>
+        </is>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>ColeAurion#2631</t>
+        </is>
+      </c>
+      <c r="AR6" t="inlineStr">
+        <is>
+          <t>Splattershot</t>
+        </is>
+      </c>
+      <c r="AS6" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
+      <c r="AT6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="AU6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="AV6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AW6" t="inlineStr">
+        <is>
+          <t>298</t>
+        </is>
+      </c>
+      <c r="AX6" t="inlineStr">
+        <is>
+          <t>Crummy#3603</t>
+        </is>
+      </c>
+      <c r="AY6" t="inlineStr">
+        <is>
+          <t>Ballpoint Splatling</t>
+        </is>
+      </c>
+      <c r="AZ6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BA6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BB6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="BC6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>1283</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>KuroOkami☆#1988</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>Dark Tetra Dualies</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>118</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>Pinec∅ne#1756</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>Painbrush</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>1008</t>
-        </is>
-      </c>
-      <c r="AJ5" t="inlineStr">
-        <is>
-          <t>cloud#1441</t>
-        </is>
-      </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>Forge Splattershot Pro</t>
-        </is>
-      </c>
-      <c r="AL5" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="AN5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="AO5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AP5" t="inlineStr">
-        <is>
-          <t>1368</t>
-        </is>
-      </c>
-      <c r="AQ5" t="inlineStr">
-        <is>
-          <t>Deliva#2529</t>
-        </is>
-      </c>
-      <c r="AR5" t="inlineStr">
-        <is>
-          <t>Flingza Roller</t>
-        </is>
-      </c>
-      <c r="AS5" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-      <c r="AT5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="AU5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="AV5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="AW5" t="inlineStr">
-        <is>
-          <t>899</t>
-        </is>
-      </c>
-      <c r="AX5" t="inlineStr">
-        <is>
-          <t>Dpsquirtle#1325</t>
-        </is>
-      </c>
-      <c r="AY5" t="inlineStr">
-        <is>
-          <t>Snipewriter 5H</t>
-        </is>
-      </c>
-      <c r="AZ5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BA5" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="BB5" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="BC5" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="BD5" t="inlineStr">
-        <is>
-          <t>1076</t>
-        </is>
-      </c>
-      <c r="BE5" t="inlineStr">
-        <is>
-          <t>BigMan#3275</t>
-        </is>
-      </c>
-      <c r="BF5" t="inlineStr">
-        <is>
-          <t>Splattershot</t>
-        </is>
-      </c>
-      <c r="BG5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BH5" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="BI5" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="BJ5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="BK5" t="inlineStr">
-        <is>
-          <t>1236</t>
+      <c r="BD6" t="inlineStr">
+        <is>
+          <t>345</t>
         </is>
       </c>
     </row>

</xml_diff>